<commit_message>
Added pull request and merge request screenshots
</commit_message>
<xml_diff>
--- a/ETS_Challenge_Screenshots.xlsx
+++ b/ETS_Challenge_Screenshots.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User\SanketM\Dev\Github\ETS_challenge\ETS_challenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1B1E9F5-5AC5-4825-8F30-21EE646B628D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA2C276-5140-4250-9920-3BB5D1404638}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="4" xr2:uid="{9008430B-71CC-482D-84F9-DC9AEC9596F5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="5" xr2:uid="{9008430B-71CC-482D-84F9-DC9AEC9596F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Visual Studio Build Error 1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="Running Code with Debugger" sheetId="3" r:id="rId3"/>
     <sheet name="Running code with debugger 2" sheetId="4" r:id="rId4"/>
     <sheet name="Result" sheetId="5" r:id="rId5"/>
+    <sheet name="Pull Request Generated Online" sheetId="6" r:id="rId6"/>
+    <sheet name="Merge Branches into Main" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -318,6 +320,104 @@
         <a:xfrm>
           <a:off x="0" y="0"/>
           <a:ext cx="18285714" cy="10285714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>1268</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>713</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F58CCA04-DC42-4CA3-856F-6393FD277B78}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="14631668" cy="8230313"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>1268</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>713</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ABF184E8-B9DF-4E33-B77E-A7269034B9F7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="14631668" cy="8230313"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -680,6 +780,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8476CE66-30A0-46AF-A6E5-5897F6D047EF}">
   <dimension ref="A1"/>
   <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EADBC9FC-ECCE-4217-8062-6D53B8F1321F}">
+  <dimension ref="A1"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -689,7 +802,35 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C605CCCB-2AC6-4E0D-A8EB-A1C81EAF62B5}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FE507CB326FB8A468257B856495989B0" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bb35377010eaa25f1ec112a1f50f322f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="210e3ef6-d63d-4dcb-9944-e63b9315733e" xmlns:ns4="90272a89-a59a-4173-8869-3a97cd689723" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f9a6a6045dd56b467868aa1415c22bda" ns3:_="" ns4:_="">
     <xsd:import namespace="210e3ef6-d63d-4dcb-9944-e63b9315733e"/>
@@ -860,22 +1001,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24115953-250C-4621-8FF3-5A83C349876A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="90272a89-a59a-4173-8869-3a97cd689723"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="210e3ef6-d63d-4dcb-9944-e63b9315733e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6777E250-B6E4-4C5A-915D-2252F05C7723}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{811BF22E-E1B1-4CA9-BC43-2CF17AA12621}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -892,29 +1043,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6777E250-B6E4-4C5A-915D-2252F05C7723}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24115953-250C-4621-8FF3-5A83C349876A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="90272a89-a59a-4173-8869-3a97cd689723"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="210e3ef6-d63d-4dcb-9944-e63b9315733e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>